<commit_message>
meeting participation percentage added
</commit_message>
<xml_diff>
--- a/template files/Add_meeting_participations.xlsx
+++ b/template files/Add_meeting_participations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs\smartiepants\template files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5182EBD-FC09-455C-BF7D-C69C0D9174F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7639C3A7-BA01-4685-B5BF-F6ACCF1335BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{19FB6BF2-D526-4AEF-8C69-EDD781109E37}"/>
+    <workbookView xWindow="2898" yWindow="2898" windowWidth="17280" windowHeight="8994" xr2:uid="{19FB6BF2-D526-4AEF-8C69-EDD781109E37}"/>
   </bookViews>
   <sheets>
     <sheet name="Participation Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="14">
   <si>
     <t>Member ID</t>
   </si>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A825825-06CE-4CEB-830E-53091FDC370B}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -450,114 +450,386 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
email sending functionality added
</commit_message>
<xml_diff>
--- a/template files/Add_meeting_participations.xlsx
+++ b/template files/Add_meeting_participations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programs\smartiepants\template files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7639C3A7-BA01-4685-B5BF-F6ACCF1335BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A31411-E59D-46D5-8F57-99647F4B7A2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2898" yWindow="2898" windowWidth="17280" windowHeight="8994" xr2:uid="{19FB6BF2-D526-4AEF-8C69-EDD781109E37}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{19FB6BF2-D526-4AEF-8C69-EDD781109E37}"/>
   </bookViews>
   <sheets>
     <sheet name="Participation Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Member ID</t>
   </si>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A825825-06CE-4CEB-830E-53091FDC370B}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -450,386 +450,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
         <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31">
-        <v>31</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35">
-        <v>35</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36">
-        <v>36</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39">
-        <v>39</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40">
-        <v>40</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41">
-        <v>41</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42">
-        <v>42</v>
-      </c>
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43">
-        <v>43</v>
-      </c>
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44">
-        <v>44</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45">
-        <v>45</v>
-      </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46">
-        <v>46</v>
-      </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47">
-        <v>47</v>
-      </c>
-      <c r="C47" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48">
-        <v>48</v>
-      </c>
-      <c r="C48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49">
-        <v>49</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>